<commit_message>
Added Brent vs Urals Crude Oil Price Chart
</commit_message>
<xml_diff>
--- a/react_app/src/datasets/urals_crude_oil.xlsx
+++ b/react_app/src/datasets/urals_crude_oil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\DataAnalysis\OilyWorld\react_app\src\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D110AE-7DC7-40E1-B71E-AAB5A5226D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C39023-C44E-4291-918C-3FDCCA1FB4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="-14850" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="-9270" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>B_Price</t>
+  </si>
+  <si>
+    <t>B_Open</t>
+  </si>
+  <si>
+    <t>B_High</t>
+  </si>
+  <si>
+    <t>B_Low</t>
   </si>
 </sst>
 </file>
@@ -120,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -147,6 +159,15 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -429,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +465,7 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -460,8 +481,20 @@
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44743</v>
       </c>
@@ -477,8 +510,20 @@
       <c r="E2" s="3">
         <v>89.53</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>99.84</v>
+      </c>
+      <c r="G2" s="10">
+        <v>109.56</v>
+      </c>
+      <c r="H2" s="10">
+        <v>114.71</v>
+      </c>
+      <c r="I2" s="10">
+        <v>98.52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44713</v>
       </c>
@@ -494,8 +539,20 @@
       <c r="E3" s="3">
         <v>94.53</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>109.03</v>
+      </c>
+      <c r="G3" s="10">
+        <v>113.14</v>
+      </c>
+      <c r="H3" s="10">
+        <v>121.74</v>
+      </c>
+      <c r="I3" s="10">
+        <v>104.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44682</v>
       </c>
@@ -511,8 +568,20 @@
       <c r="E4" s="3">
         <v>78.08</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="4">
+        <v>115.6</v>
+      </c>
+      <c r="G4" s="10">
+        <v>104.53</v>
+      </c>
+      <c r="H4" s="10">
+        <v>120.8</v>
+      </c>
+      <c r="I4" s="10">
+        <v>100.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44652</v>
       </c>
@@ -528,8 +597,20 @@
       <c r="E5" s="3">
         <v>81.83</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="4">
+        <v>107.14</v>
+      </c>
+      <c r="G5" s="10">
+        <v>103.31</v>
+      </c>
+      <c r="H5" s="10">
+        <v>113.61</v>
+      </c>
+      <c r="I5" s="10">
+        <v>97.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44621</v>
       </c>
@@ -545,8 +626,20 @@
       <c r="E6" s="3">
         <v>98.29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <v>104.71</v>
+      </c>
+      <c r="G6" s="10">
+        <v>95.48</v>
+      </c>
+      <c r="H6" s="10">
+        <v>134.91</v>
+      </c>
+      <c r="I6" s="10">
+        <v>94.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44593</v>
       </c>
@@ -562,8 +655,20 @@
       <c r="E7" s="3">
         <v>90.47</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="4">
+        <v>97.97</v>
+      </c>
+      <c r="G7" s="10">
+        <v>88.22</v>
+      </c>
+      <c r="H7" s="10">
+        <v>102.26</v>
+      </c>
+      <c r="I7" s="10">
+        <v>86.31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44562</v>
       </c>
@@ -579,8 +684,20 @@
       <c r="E8" s="3">
         <v>76.61</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="4">
+        <v>89.26</v>
+      </c>
+      <c r="G8" s="10">
+        <v>77.75</v>
+      </c>
+      <c r="H8" s="10">
+        <v>90.27</v>
+      </c>
+      <c r="I8" s="10">
+        <v>76.599999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44531</v>
       </c>
@@ -596,8 +713,20 @@
       <c r="E9" s="3">
         <v>70.55</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="4">
+        <v>77.349999999999994</v>
+      </c>
+      <c r="G9" s="10">
+        <v>69.37</v>
+      </c>
+      <c r="H9" s="10">
+        <v>80.03</v>
+      </c>
+      <c r="I9" s="10">
+        <v>65.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44501</v>
       </c>
@@ -613,8 +742,20 @@
       <c r="E10" s="3">
         <v>83.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>69.23</v>
+      </c>
+      <c r="G10" s="10">
+        <v>82.44</v>
+      </c>
+      <c r="H10" s="10">
+        <v>84.26</v>
+      </c>
+      <c r="I10" s="10">
+        <v>67.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44470</v>
       </c>
@@ -630,8 +771,20 @@
       <c r="E11" s="3">
         <v>76.67</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="4">
+        <v>83.72</v>
+      </c>
+      <c r="G11" s="10">
+        <v>77.67</v>
+      </c>
+      <c r="H11" s="10">
+        <v>85.77</v>
+      </c>
+      <c r="I11" s="10">
+        <v>76.78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44440</v>
       </c>
@@ -647,8 +800,20 @@
       <c r="E12" s="3">
         <v>68.680000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="4">
+        <v>78.31</v>
+      </c>
+      <c r="G12" s="10">
+        <v>70.98</v>
+      </c>
+      <c r="H12" s="10">
+        <v>79.95</v>
+      </c>
+      <c r="I12" s="10">
+        <v>69.849999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44409</v>
       </c>
@@ -664,8 +829,20 @@
       <c r="E13" s="3">
         <v>71.430000000000007</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>71.63</v>
+      </c>
+      <c r="G13" s="10">
+        <v>74.45</v>
+      </c>
+      <c r="H13" s="10">
+        <v>74.52</v>
+      </c>
+      <c r="I13" s="10">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44378</v>
       </c>
@@ -681,8 +858,20 @@
       <c r="E14" s="3">
         <v>74.66</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="4">
+        <v>75.41</v>
+      </c>
+      <c r="G14" s="10">
+        <v>73.83</v>
+      </c>
+      <c r="H14" s="10">
+        <v>76.8</v>
+      </c>
+      <c r="I14" s="10">
+        <v>66.91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44348</v>
       </c>
@@ -698,8 +887,20 @@
       <c r="E15" s="3">
         <v>68.81</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="4">
+        <v>74.62</v>
+      </c>
+      <c r="G15" s="10">
+        <v>69.069999999999993</v>
+      </c>
+      <c r="H15" s="10">
+        <v>75.77</v>
+      </c>
+      <c r="I15" s="10">
+        <v>68.98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44317</v>
       </c>
@@ -715,8 +916,20 @@
       <c r="E16" s="3">
         <v>68.44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="4">
+        <v>68.95</v>
+      </c>
+      <c r="G16" s="10">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="H16" s="10">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="I16" s="10">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44287</v>
       </c>
@@ -732,8 +945,20 @@
       <c r="E17" s="3">
         <v>60.35</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="4">
+        <v>66.760000000000005</v>
+      </c>
+      <c r="G17" s="10">
+        <v>62.68</v>
+      </c>
+      <c r="H17" s="10">
+        <v>68.44</v>
+      </c>
+      <c r="I17" s="10">
+        <v>60.93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44256</v>
       </c>
@@ -749,8 +974,20 @@
       <c r="E18" s="3">
         <v>64.55</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>62.74</v>
+      </c>
+      <c r="G18" s="10">
+        <v>64</v>
+      </c>
+      <c r="H18" s="10">
+        <v>70.67</v>
+      </c>
+      <c r="I18" s="10">
+        <v>60.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44228</v>
       </c>
@@ -766,8 +1003,20 @@
       <c r="E19" s="3">
         <v>56.45</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="4">
+        <v>64.42</v>
+      </c>
+      <c r="G19" s="10">
+        <v>54.7</v>
+      </c>
+      <c r="H19" s="10">
+        <v>66.819999999999993</v>
+      </c>
+      <c r="I19" s="10">
+        <v>54.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44197</v>
       </c>
@@ -783,8 +1032,20 @@
       <c r="E20" s="3">
         <v>50.97</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="4">
+        <v>55.04</v>
+      </c>
+      <c r="G20" s="10">
+        <v>51.53</v>
+      </c>
+      <c r="H20" s="10">
+        <v>57.31</v>
+      </c>
+      <c r="I20" s="10">
+        <v>50.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44166</v>
       </c>
@@ -800,8 +1061,20 @@
       <c r="E21" s="3">
         <v>49.68</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="4">
+        <v>51.82</v>
+      </c>
+      <c r="G21" s="10">
+        <v>47.95</v>
+      </c>
+      <c r="H21" s="10">
+        <v>52.46</v>
+      </c>
+      <c r="I21" s="10">
+        <v>46.81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44136</v>
       </c>
@@ -817,8 +1090,20 @@
       <c r="E22" s="3">
         <v>46.92</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="4">
+        <v>47.88</v>
+      </c>
+      <c r="G22" s="10">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="H22" s="10">
+        <v>49</v>
+      </c>
+      <c r="I22" s="10">
+        <v>36.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>44105</v>
       </c>
@@ -834,8 +1119,20 @@
       <c r="E23" s="9">
         <v>37.119999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="2">
+        <v>37.94</v>
+      </c>
+      <c r="G23" s="10">
+        <v>42.65</v>
+      </c>
+      <c r="H23" s="10">
+        <v>43.99</v>
+      </c>
+      <c r="I23" s="10">
+        <v>37.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44075</v>
       </c>
@@ -851,6 +1148,24 @@
       <c r="E24" s="3">
         <v>40.49</v>
       </c>
+      <c r="F24" s="2">
+        <v>42.3</v>
+      </c>
+      <c r="G24" s="10">
+        <v>45.96</v>
+      </c>
+      <c r="H24" s="10">
+        <v>46.57</v>
+      </c>
+      <c r="I24" s="10">
+        <v>39.880000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>